<commit_message>
Lookup Excercise & solution
</commit_message>
<xml_diff>
--- a/8. Advance Filters/Advanced+Filters.xlsx
+++ b/8. Advance Filters/Advanced+Filters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Advance_Excel_BI\8. Advance Filters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE99285-4EF1-43C2-8A56-4D3A61C72BDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12246965-1BB8-410B-803F-6C2C14DA7930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="4" xr2:uid="{29745A60-A6D0-4A7B-AF84-F627A3EF9D41}"/>
   </bookViews>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10501" uniqueCount="636">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10510" uniqueCount="636">
   <si>
     <t>Product ID</t>
   </si>
@@ -37571,10 +37571,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36F754B-9BCA-44B9-BC19-676D48331102}">
-  <dimension ref="A1:R299"/>
+  <dimension ref="A1:U299"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:N6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -37590,7 +37590,7 @@
     <col min="9" max="9" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -37619,7 +37619,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -37658,7 +37658,7 @@
       <c r="Q2" s="17"/>
       <c r="R2" s="17"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>15</v>
       </c>
@@ -37691,7 +37691,7 @@
       <c r="M3" s="24"/>
       <c r="N3" s="25"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>20</v>
       </c>
@@ -37724,7 +37724,7 @@
       <c r="M4" s="24"/>
       <c r="N4" s="25"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
@@ -37757,7 +37757,7 @@
       <c r="M5" s="24"/>
       <c r="N5" s="25"/>
     </row>
-    <row r="6" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>27</v>
       </c>
@@ -37790,7 +37790,7 @@
       <c r="M6" s="27"/>
       <c r="N6" s="28"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>30</v>
       </c>
@@ -37819,7 +37819,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>33</v>
       </c>
@@ -37847,8 +37847,35 @@
       <c r="I8" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="M8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>36</v>
       </c>
@@ -37877,7 +37904,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>40</v>
       </c>
@@ -37906,7 +37933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>43</v>
       </c>
@@ -37935,7 +37962,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
         <v>46</v>
       </c>
@@ -37964,7 +37991,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>48</v>
       </c>
@@ -37993,7 +38020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>50</v>
       </c>
@@ -38022,7 +38049,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>52</v>
       </c>
@@ -38051,7 +38078,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>55</v>
       </c>

</xml_diff>